<commit_message>
Added the beginning of a JSON file generated from original excel document :pencil:
</commit_message>
<xml_diff>
--- a/raw_released_data.xlsx
+++ b/raw_released_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex\Documents\alc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7267877-5A3D-44E2-8378-F715606ECBD3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE49353-3A09-48C3-AB73-EBD46B8BDDDB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{AC0BD6E1-1E93-43A4-8FE7-90504166469E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{AC0BD6E1-1E93-43A4-8FE7-90504166469E}"/>
   </bookViews>
   <sheets>
     <sheet name="FROSH SURVEY RESULTS, 2012-2018" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="222">
   <si>
     <t>Total Enrolled Frosh</t>
   </si>
@@ -153,12 +153,6 @@
     <t>"During the past two weeks, how many times have you had four or more drinks in a row within a 2-hour period?", Only MAAB</t>
   </si>
   <si>
-    <t>"Please mark which of the following best matches your current situation."</t>
-  </si>
-  <si>
-    <t>"Please mark which of the following best matches your current situation.": Total Respondents</t>
-  </si>
-  <si>
     <t>I am currently trying to drink alcohol in a healthier and safer way.</t>
   </si>
   <si>
@@ -186,9 +180,6 @@
     <t>"How important to you is each of the following reasons for drinking alcoholic beverages?" (%)</t>
   </si>
   <si>
-    <t>"How important to you is each of the following reasons for drinking alcoholic beverages?": Total Respondents</t>
-  </si>
-  <si>
     <t>To have a good time with your friends</t>
   </si>
   <si>
@@ -303,9 +294,6 @@
     <t>I've had problems with alcohol use in the past</t>
   </si>
   <si>
-    <t>"When you choose not to drink alcohol, how important are the following reasons?": Total Respondents</t>
-  </si>
-  <si>
     <t>"When you drink, to what degree do you do the following?"</t>
   </si>
   <si>
@@ -393,9 +381,6 @@
     <t>"When you drink, to what degree do you do the following?" (%)</t>
   </si>
   <si>
-    <t>"When you drink, to what degree do you do the following?": Total Respondents</t>
-  </si>
-  <si>
     <t>"During the past two weeks, to what degree did the following happen to you when drinking or as a result of your drinking? Don't count things that have happened to you but were not because of drinking." (%)</t>
   </si>
   <si>
@@ -459,9 +444,6 @@
     <t>Drove after drinking 5 or more drinks</t>
   </si>
   <si>
-    <t>"During the past two weeks, to what degree did the following happen to you when drinking or as a result of your drinking? Don't count things that have happened to you but were not because of drinking.": Total Respondents</t>
-  </si>
-  <si>
     <t>Data from separate graphs in data release with more precision</t>
   </si>
   <si>
@@ -477,9 +459,6 @@
     <t>Reduce the number of drinks you have each time you drink?</t>
   </si>
   <si>
-    <t>"During the next 30 days to what degree do you plan to…": Total Respondents</t>
-  </si>
-  <si>
     <t>The AlcoholEdu data is collected from two surveys administered to first-year students only, at two points: 1) pre-matriculation in August prior to the beginning of classes; and 2) post-matriculation between September and December afer students have arrived on campus. This report utilizes data from the postmatriculation survey from 2011-12 to 2017-18. Note that data from 2014-2015 is not available because a different educational platform was used that year. There are a number of limitations to the data, it should be viewed and interpreted with caution and discretion. The data is from frosh students and only during the fall quarter; no other undergraduate or graduate students were included. All data used in this analysis is based on self-reports and can be subject to social desirability bias (e.g. under/over reporting drinking behaviors to fit social norms). Some of the survey data presented here breaks down results in binary gender or sex categories. We recognize this is a shortcoming and is not inclusive of all students at Stanford. AlcoholEdu asks participants about unwanted sexual contact and alcohol. This data is included to ensure transparency in sharing all the data that is collected. It is critical that alcohol use and sexual violence are not conflated in ways that blame victims.</t>
   </si>
   <si>
@@ -507,9 +486,6 @@
     <t>Average Number of Drinks per Week (%)</t>
   </si>
   <si>
-    <t>Average Number of Drinks per Week: Total Respondents</t>
-  </si>
-  <si>
     <t>15+</t>
   </si>
   <si>
@@ -543,9 +519,6 @@
     <t>I am a non-drinker</t>
   </si>
   <si>
-    <t>Binge Drinking in Past Two Weeks: Total Respondents</t>
-  </si>
-  <si>
     <t>&lt;0.7</t>
   </si>
   <si>
@@ -591,9 +564,6 @@
     <t>"During the two weeks, have you consumed alcohol (i.e., had more than a few sips of beer, wine, or liquor)?" (%)</t>
   </si>
   <si>
-    <t>"During the past year, have you consumed alcohol (i.e., had more than a few sips of beer, wine, or liquor)?": Total Responces</t>
-  </si>
-  <si>
     <t>20+</t>
   </si>
   <si>
@@ -624,24 +594,15 @@
     <t>Graph ambiguous in which percentages apply, assigned by inspection</t>
   </si>
   <si>
-    <t>Hangover in Previous 30 Days: Total Respondents</t>
-  </si>
-  <si>
     <t>Vomiting in Previous 30 Days (%)</t>
   </si>
   <si>
-    <t>Vomiting in Previous 30 Days: Total Respondents</t>
-  </si>
-  <si>
     <t>Note that student responses from 2017 to 2018 are blank if respondents indicated having zero drinks per week in a previous question and therefore did not see this question.</t>
   </si>
   <si>
     <t>Memory Loss in Previous 30 Days (%)</t>
   </si>
   <si>
-    <t>Memory Loss in Previous 30 Days: Total Respondents</t>
-  </si>
-  <si>
     <t>Not labeled. “10+ times” was among available responses and represented 0.1% 2016 and 2017 only. Other years assumed to be 0%</t>
   </si>
   <si>
@@ -709,6 +670,36 @@
   </si>
   <si>
     <t>Number of Alcohol-Related Emergency Room Student Cases in Per Quarter, based on OAPE Data. Figures are collected on a weekly basis from police reports and/or Residence Dean on-call reports</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>2012</t>
+  </si>
+  <si>
+    <t>2013</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>Options</t>
+  </si>
+  <si>
+    <t>Total Responces</t>
   </si>
 </sst>
 </file>
@@ -744,15 +735,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1071,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B93501D-9FFD-431F-A6B0-5767EF8CA38F}">
   <dimension ref="A1:I142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="A127" sqref="A127"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,10 +1075,10 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B1" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1107,7 +1099,7 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1308,7 +1300,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="B14" t="s">
         <v>19</v>
@@ -1334,7 +1326,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="B15" t="s">
         <v>20</v>
@@ -1360,7 +1352,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
@@ -1386,7 +1378,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>185</v>
+        <v>174</v>
+      </c>
+      <c r="B17" t="s">
+        <v>221</v>
       </c>
       <c r="C17">
         <v>1326</v>
@@ -1409,7 +1404,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
@@ -1435,7 +1430,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
@@ -1461,7 +1456,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="B20" t="s">
         <v>12</v>
@@ -1751,7 +1746,7 @@
         <v>565</v>
       </c>
       <c r="I33" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -1972,10 +1967,10 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C43">
         <v>20</v>
@@ -1998,10 +1993,10 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C44">
         <v>4</v>
@@ -2024,10 +2019,10 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C45">
         <v>10</v>
@@ -2050,10 +2045,10 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C46">
         <v>66</v>
@@ -2076,7 +2071,10 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>40</v>
+        <v>43</v>
+      </c>
+      <c r="B47" t="s">
+        <v>8</v>
       </c>
       <c r="C47">
         <v>815</v>
@@ -2099,10 +2097,10 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C48">
         <v>72</v>
@@ -2123,15 +2121,15 @@
         <v>71</v>
       </c>
       <c r="I48" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
         <v>49</v>
-      </c>
-      <c r="B49" t="s">
-        <v>52</v>
       </c>
       <c r="C49">
         <v>65</v>
@@ -2154,10 +2152,10 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B50" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C50">
         <v>41</v>
@@ -2180,10 +2178,10 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B51" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C51">
         <v>38</v>
@@ -2206,10 +2204,10 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B52" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C52">
         <v>43</v>
@@ -2232,10 +2230,10 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B53" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C53">
         <v>40</v>
@@ -2258,10 +2256,10 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B54" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C54">
         <v>30</v>
@@ -2284,10 +2282,10 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B55" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C55">
         <v>33</v>
@@ -2310,10 +2308,10 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B56" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C56">
         <v>23</v>
@@ -2336,19 +2334,19 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B57" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C57" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D57" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E57" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F57">
         <v>19</v>
@@ -2362,10 +2360,10 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B58" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C58">
         <v>23</v>
@@ -2388,10 +2386,10 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B59" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C59">
         <v>13</v>
@@ -2414,7 +2412,10 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+      <c r="B60" t="s">
+        <v>8</v>
       </c>
       <c r="C60">
         <v>813</v>
@@ -2437,10 +2438,10 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C61">
         <v>70</v>
@@ -2463,10 +2464,10 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C62">
         <v>66</v>
@@ -2489,10 +2490,10 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B63" t="s">
         <v>64</v>
-      </c>
-      <c r="B63" t="s">
-        <v>67</v>
       </c>
       <c r="C63">
         <v>62</v>
@@ -2515,10 +2516,10 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B64" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C64">
         <v>67</v>
@@ -2541,10 +2542,10 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B65" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C65">
         <v>48</v>
@@ -2567,10 +2568,10 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B66" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C66">
         <v>50</v>
@@ -2593,10 +2594,10 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B67" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C67">
         <v>56</v>
@@ -2619,10 +2620,10 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B68" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C68">
         <v>44</v>
@@ -2645,10 +2646,10 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B69" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C69">
         <v>32</v>
@@ -2671,10 +2672,10 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B70" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C70">
         <v>40</v>
@@ -2697,10 +2698,10 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B71" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C71">
         <v>28</v>
@@ -2723,10 +2724,10 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B72" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C72">
         <v>41</v>
@@ -2749,10 +2750,10 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B73" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C73">
         <v>37</v>
@@ -2775,10 +2776,10 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B74" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C74">
         <v>38</v>
@@ -2801,10 +2802,10 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B75" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C75">
         <v>31</v>
@@ -2827,10 +2828,10 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B76" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C76">
         <v>30</v>
@@ -2853,10 +2854,10 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B77" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C77">
         <v>27</v>
@@ -2879,10 +2880,10 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B78" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C78">
         <v>19</v>
@@ -2905,10 +2906,10 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B79" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C79">
         <v>22</v>
@@ -2931,10 +2932,10 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B80" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C80">
         <v>20</v>
@@ -2957,10 +2958,10 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B81" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C81">
         <v>16</v>
@@ -2983,10 +2984,10 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B82" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C82">
         <v>11</v>
@@ -3009,10 +3010,10 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B83" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C83">
         <v>9</v>
@@ -3035,10 +3036,10 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B84" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C84">
         <v>7</v>
@@ -3061,7 +3062,10 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>89</v>
+        <v>61</v>
+      </c>
+      <c r="B85" t="s">
+        <v>8</v>
       </c>
       <c r="C85">
         <v>1280</v>
@@ -3084,10 +3088,10 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B86" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C86">
         <v>802</v>
@@ -3108,15 +3112,15 @@
         <v>708</v>
       </c>
       <c r="I86" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C87">
         <v>803</v>
@@ -3139,10 +3143,10 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C88">
         <v>795</v>
@@ -3165,10 +3169,10 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>86</v>
+      </c>
+      <c r="B89" t="s">
         <v>90</v>
-      </c>
-      <c r="B89" t="s">
-        <v>94</v>
       </c>
       <c r="C89">
         <v>801</v>
@@ -3191,10 +3195,10 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B90" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C90">
         <v>803</v>
@@ -3217,10 +3221,10 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B91" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C91">
         <v>85</v>
@@ -3241,15 +3245,15 @@
         <v>88</v>
       </c>
       <c r="I91" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B92" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C92">
         <v>78</v>
@@ -3272,10 +3276,10 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B93" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C93">
         <v>78</v>
@@ -3298,10 +3302,10 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B94" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C94">
         <v>61</v>
@@ -3324,10 +3328,10 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B95" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C95">
         <v>71</v>
@@ -3350,10 +3354,10 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B96" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C96">
         <v>74</v>
@@ -3376,10 +3380,10 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B97" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C97">
         <v>58</v>
@@ -3402,10 +3406,10 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B98" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C98">
         <v>71</v>
@@ -3428,10 +3432,10 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B99" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C99">
         <v>62</v>
@@ -3454,10 +3458,10 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B100" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C100">
         <v>56</v>
@@ -3480,10 +3484,10 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B101" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C101">
         <v>52</v>
@@ -3506,10 +3510,10 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B102" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C102">
         <v>38</v>
@@ -3532,10 +3536,10 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B103" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C103">
         <v>52</v>
@@ -3558,10 +3562,10 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B104" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C104">
         <v>35</v>
@@ -3584,10 +3588,10 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B105" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C105">
         <v>39</v>
@@ -3610,10 +3614,10 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B106" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C106">
         <v>37</v>
@@ -3636,10 +3640,10 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B107" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C107">
         <v>36</v>
@@ -3662,10 +3666,10 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B108" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C108">
         <v>33</v>
@@ -3688,10 +3692,10 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B109" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C109">
         <v>22</v>
@@ -3714,10 +3718,10 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B110" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C110">
         <v>24</v>
@@ -3740,10 +3744,10 @@
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B111" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C111">
         <v>21</v>
@@ -3766,7 +3770,10 @@
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>119</v>
+        <v>114</v>
+      </c>
+      <c r="B112" t="s">
+        <v>8</v>
       </c>
       <c r="C112">
         <v>809</v>
@@ -3789,10 +3796,10 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B113" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C113">
         <v>37</v>
@@ -3813,15 +3820,15 @@
         <v>38</v>
       </c>
       <c r="I113" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B114" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C114">
         <v>33</v>
@@ -3844,10 +3851,10 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B115" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C115">
         <v>36</v>
@@ -3870,10 +3877,10 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C116">
         <v>39</v>
@@ -3896,10 +3903,10 @@
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
+        <v>115</v>
+      </c>
+      <c r="B117" t="s">
         <v>120</v>
-      </c>
-      <c r="B117" t="s">
-        <v>125</v>
       </c>
       <c r="C117">
         <v>32</v>
@@ -3922,10 +3929,10 @@
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B118" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C118">
         <v>14</v>
@@ -3948,10 +3955,10 @@
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B119" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C119">
         <v>18</v>
@@ -3974,10 +3981,10 @@
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B120" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C120">
         <v>12</v>
@@ -4000,10 +4007,10 @@
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B121" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C121">
         <v>16</v>
@@ -4026,10 +4033,10 @@
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B122" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C122">
         <v>12</v>
@@ -4052,10 +4059,10 @@
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B123" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C123">
         <v>11.6</v>
@@ -4076,15 +4083,15 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="I123" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B124" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C124">
         <v>12</v>
@@ -4107,10 +4114,10 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B125" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C125">
         <v>5</v>
@@ -4133,10 +4140,10 @@
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B126" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C126">
         <v>5</v>
@@ -4159,10 +4166,10 @@
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B127" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C127">
         <v>6</v>
@@ -4185,10 +4192,10 @@
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B128" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C128">
         <v>4</v>
@@ -4211,10 +4218,10 @@
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B129" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C129">
         <v>3</v>
@@ -4237,10 +4244,10 @@
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B130" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C130">
         <v>5.9</v>
@@ -4261,15 +4268,15 @@
         <v>3.2</v>
       </c>
       <c r="I130" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B131" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C131">
         <v>5</v>
@@ -4292,10 +4299,10 @@
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B132" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C132">
         <v>4</v>
@@ -4318,7 +4325,10 @@
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>141</v>
+        <v>115</v>
+      </c>
+      <c r="B133" t="s">
+        <v>8</v>
       </c>
       <c r="C133">
         <v>670</v>
@@ -4341,10 +4351,10 @@
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B134" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F134">
         <v>50</v>
@@ -4356,15 +4366,15 @@
         <v>55</v>
       </c>
       <c r="I134" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B135" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F135">
         <v>47</v>
@@ -4378,10 +4388,10 @@
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B136" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F136">
         <v>24</v>
@@ -4395,10 +4405,10 @@
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B137" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="F137">
         <v>18</v>
@@ -4412,10 +4422,10 @@
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B138" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="F138">
         <v>18</v>
@@ -4429,7 +4439,10 @@
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>147</v>
+        <v>138</v>
+      </c>
+      <c r="B139" t="s">
+        <v>8</v>
       </c>
       <c r="F139">
         <v>700</v>
@@ -4443,7 +4456,7 @@
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -4455,1263 +4468,1285 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CFAE440-41FB-4F7D-B135-076641C121EA}">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="55" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="2"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3" s="2">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="D3" s="2">
+        <v>39.6</v>
+      </c>
+      <c r="E3" s="2">
+        <v>41.3</v>
+      </c>
+      <c r="F3" s="2">
+        <v>34.1</v>
+      </c>
+      <c r="G3" s="2">
+        <v>41.7</v>
+      </c>
+      <c r="H3" s="2">
+        <v>39.4</v>
+      </c>
+      <c r="I3" s="2">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>58.7</v>
+      </c>
+      <c r="D4" s="2">
+        <v>59.3</v>
+      </c>
+      <c r="E4" s="2">
+        <v>58.4</v>
+      </c>
+      <c r="F4" s="2">
+        <v>64.7</v>
+      </c>
+      <c r="G4" s="2">
+        <v>57.1</v>
+      </c>
+      <c r="H4" s="2">
+        <v>30.8</v>
+      </c>
+      <c r="I4" s="2">
+        <v>32.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
+        <v>29.8</v>
+      </c>
+      <c r="I5" s="2">
+        <v>31.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2">
+        <v>583</v>
+      </c>
+      <c r="D6" s="2">
+        <v>548</v>
+      </c>
+      <c r="E6" s="2">
+        <v>438</v>
+      </c>
+      <c r="F6" s="2">
+        <v>428</v>
+      </c>
+      <c r="G6" s="2">
+        <v>902</v>
+      </c>
+      <c r="H6" s="2">
+        <v>977</v>
+      </c>
+      <c r="I6" s="2">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B7" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C1">
-        <v>2012</v>
-      </c>
-      <c r="D1">
-        <v>2013</v>
-      </c>
-      <c r="E1">
-        <v>2014</v>
-      </c>
-      <c r="F1">
-        <v>2015</v>
-      </c>
-      <c r="G1">
-        <v>2016</v>
-      </c>
-      <c r="H1">
-        <v>2017</v>
-      </c>
-      <c r="I1">
-        <v>2018</v>
-      </c>
-      <c r="J1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C7" s="2">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2">
+        <v>4</v>
+      </c>
+      <c r="F7" s="2">
+        <v>3</v>
+      </c>
+      <c r="G7" s="2">
+        <v>5</v>
+      </c>
+      <c r="H7" s="2">
+        <v>5</v>
+      </c>
+      <c r="I7" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C8" s="2">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2">
+        <v>11</v>
+      </c>
+      <c r="E8" s="2">
+        <v>11</v>
+      </c>
+      <c r="F8" s="2">
+        <v>11</v>
+      </c>
+      <c r="G8" s="2">
+        <v>11</v>
+      </c>
+      <c r="H8" s="2">
+        <v>9</v>
+      </c>
+      <c r="I8" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C9" s="2">
+        <v>44</v>
+      </c>
+      <c r="D9" s="2">
+        <v>50</v>
+      </c>
+      <c r="E9" s="2">
+        <v>47</v>
+      </c>
+      <c r="F9" s="2">
+        <v>52</v>
+      </c>
+      <c r="G9" s="2">
+        <v>56</v>
+      </c>
+      <c r="H9" s="2">
+        <v>56</v>
+      </c>
+      <c r="I9" s="2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2">
+        <v>38</v>
+      </c>
+      <c r="D10" s="2">
+        <v>33</v>
+      </c>
+      <c r="E10" s="2">
+        <v>37</v>
+      </c>
+      <c r="F10" s="2">
+        <v>33</v>
+      </c>
+      <c r="G10" s="2">
+        <v>27</v>
+      </c>
+      <c r="H10" s="2">
+        <v>29</v>
+      </c>
+      <c r="I10" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I11" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B12" t="s">
+        <v>221</v>
+      </c>
+      <c r="C12" s="2">
+        <v>583</v>
+      </c>
+      <c r="D12" s="2">
+        <v>548</v>
+      </c>
+      <c r="E12" s="2">
+        <v>438</v>
+      </c>
+      <c r="F12" s="2">
+        <v>428</v>
+      </c>
+      <c r="G12" s="2">
+        <v>902</v>
+      </c>
+      <c r="H12" s="2">
+        <v>977</v>
+      </c>
+      <c r="I12" s="2">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G14" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F15" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="G15" s="2">
+        <v>5.3</v>
+      </c>
+      <c r="H15" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="I15" s="2">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F16" s="2">
+        <v>29</v>
+      </c>
+      <c r="G16" s="2">
+        <v>35</v>
+      </c>
+      <c r="H16" s="2">
+        <v>33</v>
+      </c>
+      <c r="I16" s="2">
+        <v>31.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F17" s="2">
+        <v>64.7</v>
+      </c>
+      <c r="G17" s="2">
+        <v>57.1</v>
+      </c>
+      <c r="H17" s="2">
+        <v>30.7</v>
+      </c>
+      <c r="I17" s="2">
+        <v>32.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G19" s="2">
+        <v>1</v>
+      </c>
+      <c r="H19" s="2">
+        <v>29.8</v>
+      </c>
+      <c r="I19" s="2">
+        <v>31.2</v>
+      </c>
+      <c r="J19" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C2">
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B20" t="s">
+        <v>221</v>
+      </c>
+      <c r="F20" s="2">
+        <v>428</v>
+      </c>
+      <c r="G20" s="2">
+        <v>902</v>
+      </c>
+      <c r="H20" s="2">
+        <v>977</v>
+      </c>
+      <c r="I20" s="2">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="H22" s="2">
         <v>0.3</v>
       </c>
-      <c r="D2">
+      <c r="I22" s="2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F23" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="G23" s="2">
+        <v>3</v>
+      </c>
+      <c r="H23" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="I23" s="2">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F24" s="2">
+        <v>24.3</v>
+      </c>
+      <c r="G24" s="2">
+        <v>25.9</v>
+      </c>
+      <c r="H24" s="2">
+        <v>25.7</v>
+      </c>
+      <c r="I24" s="2">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F25" s="2">
+        <v>70.8</v>
+      </c>
+      <c r="G25" s="2">
+        <v>69.2</v>
+      </c>
+      <c r="H25" s="2">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="I25" s="2">
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="2">
         <v>0.7</v>
       </c>
-      <c r="E2">
+      <c r="G26" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="H26" s="2">
+        <v>30.3</v>
+      </c>
+      <c r="I26" s="2">
+        <v>31.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B27" t="s">
+        <v>221</v>
+      </c>
+      <c r="F27" s="2">
+        <v>428</v>
+      </c>
+      <c r="G27" s="2">
+        <v>902</v>
+      </c>
+      <c r="H27" s="2">
+        <v>977</v>
+      </c>
+      <c r="I27" s="2">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I28" s="2">
+        <v>0</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="G29" s="2">
         <v>0.2</v>
       </c>
-      <c r="F2">
+      <c r="H29" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="I29" s="2">
+        <v>0</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F30" s="2">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="G30" s="2">
+        <v>9.6</v>
+      </c>
+      <c r="H30" s="2">
+        <v>10.3</v>
+      </c>
+      <c r="I30" s="2">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F31" s="2">
+        <v>88.6</v>
+      </c>
+      <c r="G31" s="2">
+        <v>88.9</v>
+      </c>
+      <c r="H31" s="2">
+        <v>59.4</v>
+      </c>
+      <c r="I31" s="2">
+        <v>60.7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="G32" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H32" s="2">
+        <v>30</v>
+      </c>
+      <c r="I32" s="2">
+        <v>31.4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B33" t="s">
+        <v>221</v>
+      </c>
+      <c r="F33" s="2">
+        <v>428</v>
+      </c>
+      <c r="G33" s="2">
+        <v>902</v>
+      </c>
+      <c r="H33" s="2">
+        <v>977</v>
+      </c>
+      <c r="I33" s="2">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F34" s="2">
+        <v>0</v>
+      </c>
+      <c r="G34" s="2">
+        <v>0</v>
+      </c>
+      <c r="H34" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I34" s="2">
+        <v>0</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F35" s="2">
         <v>0.7</v>
       </c>
-      <c r="G2">
-        <v>0.2</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0.2</v>
-      </c>
-      <c r="J2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>152</v>
-      </c>
-      <c r="B3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C3">
-        <v>40.299999999999997</v>
-      </c>
-      <c r="D3">
-        <v>39.6</v>
-      </c>
-      <c r="E3">
-        <v>41.3</v>
-      </c>
-      <c r="F3">
-        <v>34.1</v>
-      </c>
-      <c r="G3">
-        <v>41.7</v>
-      </c>
-      <c r="H3">
-        <v>39.4</v>
-      </c>
-      <c r="I3">
-        <v>36.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>152</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>58.7</v>
-      </c>
-      <c r="D4">
-        <v>59.3</v>
-      </c>
-      <c r="E4">
-        <v>58.4</v>
-      </c>
-      <c r="F4">
-        <v>64.7</v>
-      </c>
-      <c r="G4">
-        <v>57.1</v>
-      </c>
-      <c r="H4">
-        <v>30.8</v>
-      </c>
-      <c r="I4">
-        <v>32.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>152</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="G35" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="H35" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="I35" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F36" s="2">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="G36" s="2">
+        <v>8.9</v>
+      </c>
+      <c r="H36" s="2">
+        <v>7.8</v>
+      </c>
+      <c r="I36" s="2">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F37" s="2">
+        <v>90.4</v>
+      </c>
+      <c r="G37" s="2">
+        <v>89.7</v>
+      </c>
+      <c r="H37" s="2">
+        <v>71.7</v>
+      </c>
+      <c r="I37" s="2">
+        <v>59.4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5">
-        <v>0.7</v>
-      </c>
-      <c r="D5">
-        <v>0.4</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
+      <c r="F38" s="2">
         <v>0.5</v>
       </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>29.8</v>
-      </c>
-      <c r="I5">
-        <v>31.2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>153</v>
-      </c>
-      <c r="C6">
-        <v>583</v>
-      </c>
-      <c r="D6">
-        <v>548</v>
-      </c>
-      <c r="E6">
-        <v>438</v>
-      </c>
-      <c r="F6">
+      <c r="G38" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="H38" s="2">
+        <v>29.9</v>
+      </c>
+      <c r="I38" s="2">
+        <v>31.3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B39" t="s">
+        <v>221</v>
+      </c>
+      <c r="F39" s="2">
         <v>428</v>
       </c>
-      <c r="G6">
+      <c r="G39" s="2">
         <v>902</v>
       </c>
-      <c r="H6">
+      <c r="H39" s="2">
         <v>977</v>
       </c>
-      <c r="I6">
-        <v>825</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>156</v>
-      </c>
-      <c r="B7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-      <c r="D7">
-        <v>6</v>
-      </c>
-      <c r="E7">
-        <v>4</v>
-      </c>
-      <c r="F7">
-        <v>3</v>
-      </c>
-      <c r="G7">
-        <v>5</v>
-      </c>
-      <c r="H7">
-        <v>5</v>
-      </c>
-      <c r="I7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>156</v>
-      </c>
-      <c r="B8" t="s">
-        <v>159</v>
-      </c>
-      <c r="C8">
-        <v>12</v>
-      </c>
-      <c r="D8">
-        <v>11</v>
-      </c>
-      <c r="E8">
-        <v>11</v>
-      </c>
-      <c r="F8">
-        <v>11</v>
-      </c>
-      <c r="G8">
-        <v>11</v>
-      </c>
-      <c r="H8">
-        <v>9</v>
-      </c>
-      <c r="I8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>156</v>
-      </c>
-      <c r="B9" t="s">
-        <v>160</v>
-      </c>
-      <c r="C9">
-        <v>44</v>
-      </c>
-      <c r="D9">
-        <v>50</v>
-      </c>
-      <c r="E9">
-        <v>47</v>
-      </c>
-      <c r="F9">
-        <v>52</v>
-      </c>
-      <c r="G9">
-        <v>56</v>
-      </c>
-      <c r="H9">
-        <v>56</v>
-      </c>
-      <c r="I9">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>156</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>38</v>
-      </c>
-      <c r="D10">
-        <v>33</v>
-      </c>
-      <c r="E10">
-        <v>37</v>
-      </c>
-      <c r="F10">
-        <v>33</v>
-      </c>
-      <c r="G10">
-        <v>27</v>
-      </c>
-      <c r="H10">
-        <v>29</v>
-      </c>
-      <c r="I10">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>156</v>
-      </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>0.5</v>
-      </c>
-      <c r="I11">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>157</v>
-      </c>
-      <c r="C12">
-        <v>583</v>
-      </c>
-      <c r="D12">
-        <v>548</v>
-      </c>
-      <c r="E12">
-        <v>438</v>
-      </c>
-      <c r="F12">
-        <v>428</v>
-      </c>
-      <c r="G12">
-        <v>902</v>
-      </c>
-      <c r="H12">
-        <v>977</v>
-      </c>
-      <c r="I12">
-        <v>825</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>161</v>
-      </c>
-      <c r="B13" t="s">
-        <v>163</v>
-      </c>
-      <c r="F13" t="s">
-        <v>170</v>
-      </c>
-      <c r="G13" t="s">
-        <v>170</v>
-      </c>
-      <c r="H13" t="s">
-        <v>170</v>
-      </c>
-      <c r="I13" t="s">
-        <v>170</v>
-      </c>
-      <c r="J13" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>161</v>
-      </c>
-      <c r="B14" t="s">
-        <v>164</v>
-      </c>
-      <c r="F14">
-        <v>0.5</v>
-      </c>
-      <c r="G14">
-        <v>1.3</v>
-      </c>
-      <c r="H14">
-        <v>0.9</v>
-      </c>
-      <c r="I14">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>161</v>
-      </c>
-      <c r="B15" t="s">
-        <v>165</v>
-      </c>
-      <c r="F15">
-        <v>4.7</v>
-      </c>
-      <c r="G15">
-        <v>5.3</v>
-      </c>
-      <c r="H15">
-        <v>5.5</v>
-      </c>
-      <c r="I15">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>161</v>
-      </c>
-      <c r="B16" t="s">
-        <v>166</v>
-      </c>
-      <c r="F16">
-        <v>29</v>
-      </c>
-      <c r="G16">
-        <v>35</v>
-      </c>
-      <c r="H16">
-        <v>33</v>
-      </c>
-      <c r="I16">
-        <v>31.4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>161</v>
-      </c>
-      <c r="B17" t="s">
-        <v>167</v>
-      </c>
-      <c r="F17">
-        <v>64.7</v>
-      </c>
-      <c r="G17">
-        <v>57.1</v>
-      </c>
-      <c r="H17">
-        <v>30.7</v>
-      </c>
-      <c r="I17">
-        <v>32.1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>161</v>
-      </c>
-      <c r="B18" t="s">
-        <v>168</v>
-      </c>
-      <c r="F18" t="s">
-        <v>171</v>
-      </c>
-      <c r="G18" t="s">
-        <v>171</v>
-      </c>
-      <c r="H18">
-        <v>0.01</v>
-      </c>
-      <c r="I18" t="s">
-        <v>171</v>
-      </c>
-      <c r="J18" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>161</v>
-      </c>
-      <c r="B19" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19">
-        <v>0.5</v>
-      </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-      <c r="H19">
-        <v>29.8</v>
-      </c>
-      <c r="I19">
-        <v>31.2</v>
-      </c>
-      <c r="J19" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>169</v>
-      </c>
-      <c r="F20">
-        <v>428</v>
-      </c>
-      <c r="G20">
-        <v>902</v>
-      </c>
-      <c r="H20">
-        <v>977</v>
-      </c>
-      <c r="I20">
-        <v>825</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B21" t="s">
-        <v>179</v>
-      </c>
-      <c r="F21">
-        <v>0.5</v>
-      </c>
-      <c r="G21">
-        <v>0.4</v>
-      </c>
-      <c r="H21">
-        <v>0.4</v>
-      </c>
-      <c r="I21">
-        <v>0.2</v>
-      </c>
-      <c r="J21" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>194</v>
-      </c>
-      <c r="B22" t="s">
-        <v>164</v>
-      </c>
-      <c r="F22">
-        <v>0.2</v>
-      </c>
-      <c r="G22">
-        <v>0.6</v>
-      </c>
-      <c r="H22">
-        <v>0.3</v>
-      </c>
-      <c r="I22">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>194</v>
-      </c>
-      <c r="B23" t="s">
-        <v>165</v>
-      </c>
-      <c r="F23">
-        <v>3.5</v>
-      </c>
-      <c r="G23">
-        <v>3</v>
-      </c>
-      <c r="H23">
-        <v>2.5</v>
-      </c>
-      <c r="I23">
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>194</v>
-      </c>
-      <c r="B24" t="s">
-        <v>166</v>
-      </c>
-      <c r="F24">
-        <v>24.3</v>
-      </c>
-      <c r="G24">
-        <v>25.9</v>
-      </c>
-      <c r="H24">
-        <v>25.7</v>
-      </c>
-      <c r="I24">
-        <v>25.3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>194</v>
-      </c>
-      <c r="B25" t="s">
-        <v>167</v>
-      </c>
-      <c r="F25">
-        <v>70.8</v>
-      </c>
-      <c r="G25">
-        <v>69.2</v>
-      </c>
-      <c r="H25">
-        <v>40.799999999999997</v>
-      </c>
-      <c r="I25">
-        <v>40.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>194</v>
-      </c>
-      <c r="B26" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26">
-        <v>0.7</v>
-      </c>
-      <c r="G26">
-        <v>0.9</v>
-      </c>
-      <c r="H26">
-        <v>30.3</v>
-      </c>
-      <c r="I26">
-        <v>31.2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>196</v>
-      </c>
-      <c r="F27">
-        <v>428</v>
-      </c>
-      <c r="G27">
-        <v>902</v>
-      </c>
-      <c r="H27">
-        <v>977</v>
-      </c>
-      <c r="I27">
-        <v>825</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>197</v>
-      </c>
-      <c r="B28" t="s">
-        <v>179</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28">
-        <v>0.1</v>
-      </c>
-      <c r="H28">
-        <v>0.1</v>
-      </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>197</v>
-      </c>
-      <c r="B29" t="s">
-        <v>165</v>
-      </c>
-      <c r="F29">
-        <v>0.7</v>
-      </c>
-      <c r="G29">
-        <v>0.2</v>
-      </c>
-      <c r="H29">
-        <v>0.2</v>
-      </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
-      <c r="J29" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>197</v>
-      </c>
-      <c r="B30" t="s">
-        <v>166</v>
-      </c>
-      <c r="F30">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="G30">
-        <v>9.6</v>
-      </c>
-      <c r="H30">
-        <v>10.3</v>
-      </c>
-      <c r="I30">
-        <v>7.9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>197</v>
-      </c>
-      <c r="B31" t="s">
-        <v>167</v>
-      </c>
-      <c r="F31">
-        <v>88.6</v>
-      </c>
-      <c r="G31">
-        <v>88.9</v>
-      </c>
-      <c r="H31">
-        <v>59.4</v>
-      </c>
-      <c r="I31">
-        <v>60.7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>197</v>
-      </c>
-      <c r="B32" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32">
-        <v>0.9</v>
-      </c>
-      <c r="G32">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H32">
-        <v>30</v>
-      </c>
-      <c r="I32">
-        <v>31.4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>198</v>
-      </c>
-      <c r="F33">
-        <v>428</v>
-      </c>
-      <c r="G33">
-        <v>902</v>
-      </c>
-      <c r="H33">
-        <v>977</v>
-      </c>
-      <c r="I33">
-        <v>825</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>200</v>
-      </c>
-      <c r="B34" t="s">
-        <v>163</v>
-      </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-      <c r="H34">
-        <v>0.1</v>
-      </c>
-      <c r="I34">
-        <v>0</v>
-      </c>
-      <c r="J34" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>200</v>
-      </c>
-      <c r="B35" t="s">
-        <v>165</v>
-      </c>
-      <c r="F35">
-        <v>0.7</v>
-      </c>
-      <c r="G35">
-        <v>0.6</v>
-      </c>
-      <c r="H35">
-        <v>0.4</v>
-      </c>
-      <c r="I35">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>200</v>
-      </c>
-      <c r="B36" t="s">
-        <v>166</v>
-      </c>
-      <c r="F36">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="G36">
-        <v>8.9</v>
-      </c>
-      <c r="H36">
-        <v>7.8</v>
-      </c>
-      <c r="I36">
-        <v>8.6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>200</v>
-      </c>
-      <c r="B37" t="s">
-        <v>167</v>
-      </c>
-      <c r="F37">
-        <v>90.4</v>
-      </c>
-      <c r="G37">
-        <v>89.7</v>
-      </c>
-      <c r="H37">
-        <v>71.7</v>
-      </c>
-      <c r="I37">
-        <v>59.4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>200</v>
-      </c>
-      <c r="B38" t="s">
-        <v>12</v>
-      </c>
-      <c r="F38">
-        <v>0.5</v>
-      </c>
-      <c r="G38">
-        <v>0.8</v>
-      </c>
-      <c r="H38">
-        <v>29.9</v>
-      </c>
-      <c r="I38">
-        <v>31.3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>201</v>
-      </c>
-      <c r="F39">
-        <v>428</v>
-      </c>
-      <c r="G39">
-        <v>902</v>
-      </c>
-      <c r="H39">
-        <v>977</v>
-      </c>
-      <c r="I39">
+      <c r="I39" s="2">
         <v>825</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C41" s="3" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
-      <c r="I41" s="2"/>
+      <c r="I41" s="4"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
-        <v>173</v>
-      </c>
-      <c r="D42" t="s">
-        <v>174</v>
-      </c>
-      <c r="E42" t="s">
-        <v>175</v>
-      </c>
-      <c r="F42" t="s">
+      <c r="C42" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="E43" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="F43" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="G43" s="2">
+        <v>0</v>
+      </c>
+      <c r="H43" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C44" s="2">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="D44" s="2">
+        <v>37</v>
+      </c>
+      <c r="E44" s="2">
+        <v>41.5</v>
+      </c>
+      <c r="F44" s="2">
+        <v>43.3</v>
+      </c>
+      <c r="G44" s="2">
+        <v>26.8</v>
+      </c>
+      <c r="H44" s="2">
+        <v>30.4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C45" s="2">
+        <v>49</v>
+      </c>
+      <c r="D45" s="2">
+        <v>50.5</v>
+      </c>
+      <c r="E45" s="2">
+        <v>48</v>
+      </c>
+      <c r="F45" s="2">
+        <v>50.4</v>
+      </c>
+      <c r="G45" s="2">
+        <v>64.3</v>
+      </c>
+      <c r="H45" s="2">
+        <v>18.399999999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" s="2">
+        <v>13</v>
+      </c>
+      <c r="D46" s="2">
+        <v>12.1</v>
+      </c>
+      <c r="E46" s="2">
+        <v>10</v>
+      </c>
+      <c r="F46" s="2">
+        <v>6.1</v>
+      </c>
+      <c r="G46" s="2">
+        <v>8.9</v>
+      </c>
+      <c r="H46" s="2">
+        <v>51.3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C47" s="2">
+        <v>1317</v>
+      </c>
+      <c r="D47" s="2">
+        <v>1145</v>
+      </c>
+      <c r="E47" s="2">
+        <v>1170</v>
+      </c>
+      <c r="F47" s="2">
+        <v>855</v>
+      </c>
+      <c r="G47" s="2">
+        <v>56</v>
+      </c>
+      <c r="H47" s="2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" s="2">
+        <v>5.7</v>
+      </c>
+      <c r="D48" s="2">
+        <v>4</v>
+      </c>
+      <c r="E48" s="2">
+        <v>3</v>
+      </c>
+      <c r="F48" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="G48" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="H48" s="2">
+        <v>27.8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="G42" t="s">
+      <c r="C49" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="H42" t="s">
+      <c r="C50" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D50" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="E50" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="F50" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="H50" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>152</v>
-      </c>
-      <c r="B43" t="s">
+      <c r="C51" s="2">
+        <v>4.3</v>
+      </c>
+      <c r="D51" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="E51" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="F51" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="H51" s="2">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C43">
-        <v>0.2</v>
-      </c>
-      <c r="D43">
-        <v>0.3</v>
-      </c>
-      <c r="E43">
-        <v>0.4</v>
-      </c>
-      <c r="F43">
-        <v>0.2</v>
-      </c>
-      <c r="G43">
+      <c r="C52" s="2">
+        <v>15</v>
+      </c>
+      <c r="D52" s="2">
+        <v>13.4</v>
+      </c>
+      <c r="E52" s="2">
+        <v>15.2</v>
+      </c>
+      <c r="F52" s="2">
+        <v>18.5</v>
+      </c>
+      <c r="G52" s="2">
+        <v>12.5</v>
+      </c>
+      <c r="H52" s="2">
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C53" s="2">
+        <v>37.1</v>
+      </c>
+      <c r="D53" s="2">
+        <v>43</v>
+      </c>
+      <c r="E53" s="2">
+        <v>51.2</v>
+      </c>
+      <c r="F53" s="2">
+        <v>54</v>
+      </c>
+      <c r="G53" s="2">
+        <v>58.9</v>
+      </c>
+      <c r="H53" s="2">
+        <v>32.299999999999997</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B54" s="2">
         <v>0</v>
       </c>
-      <c r="H43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>152</v>
-      </c>
-      <c r="B44" t="s">
-        <v>180</v>
-      </c>
-      <c r="C44">
-        <v>37.799999999999997</v>
-      </c>
-      <c r="D44">
-        <v>37</v>
-      </c>
-      <c r="E44">
-        <v>41.5</v>
-      </c>
-      <c r="F44">
-        <v>43.3</v>
-      </c>
-      <c r="G44">
+      <c r="C54" s="2">
+        <v>34.9</v>
+      </c>
+      <c r="D54" s="2">
+        <v>33</v>
+      </c>
+      <c r="E54" s="2">
+        <v>24.4</v>
+      </c>
+      <c r="F54" s="2">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="G54" s="2">
         <v>26.8</v>
       </c>
-      <c r="H44">
-        <v>30.4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>152</v>
-      </c>
-      <c r="B45" t="s">
-        <v>167</v>
-      </c>
-      <c r="C45">
-        <v>49</v>
-      </c>
-      <c r="D45">
-        <v>50.5</v>
-      </c>
-      <c r="E45">
-        <v>48</v>
-      </c>
-      <c r="F45">
-        <v>50.4</v>
-      </c>
-      <c r="G45">
-        <v>64.3</v>
-      </c>
-      <c r="H45">
-        <v>18.399999999999999</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>152</v>
-      </c>
-      <c r="B46" t="s">
-        <v>12</v>
-      </c>
-      <c r="C46">
-        <v>13</v>
-      </c>
-      <c r="D46">
-        <v>12.1</v>
-      </c>
-      <c r="E46">
-        <v>10</v>
-      </c>
-      <c r="F46">
-        <v>6.1</v>
-      </c>
-      <c r="G46">
-        <v>8.9</v>
-      </c>
-      <c r="H46">
-        <v>51.3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>153</v>
-      </c>
-      <c r="C47">
+      <c r="H54" s="2">
+        <v>19.600000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C55" s="2">
         <v>1317</v>
       </c>
-      <c r="D47">
+      <c r="D55" s="2">
         <v>1145</v>
       </c>
-      <c r="E47">
+      <c r="E55" s="2">
         <v>1170</v>
       </c>
-      <c r="F47">
+      <c r="F55" s="2">
         <v>855</v>
       </c>
-      <c r="G47">
+      <c r="G55" s="2">
         <v>56</v>
       </c>
-      <c r="H47">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>156</v>
-      </c>
-      <c r="B48" t="s">
-        <v>12</v>
-      </c>
-      <c r="C48">
-        <v>5.7</v>
-      </c>
-      <c r="D48">
-        <v>4</v>
-      </c>
-      <c r="E48">
-        <v>3</v>
-      </c>
-      <c r="F48">
-        <v>2.1</v>
-      </c>
-      <c r="G48">
-        <v>1.8</v>
-      </c>
-      <c r="H48">
-        <v>27.8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>156</v>
-      </c>
-      <c r="B49" t="s">
-        <v>186</v>
-      </c>
-      <c r="C49" t="s">
-        <v>191</v>
-      </c>
-      <c r="D49" t="s">
-        <v>191</v>
-      </c>
-      <c r="E49" t="s">
-        <v>191</v>
-      </c>
-      <c r="F49" t="s">
-        <v>191</v>
-      </c>
-      <c r="G49" t="s">
-        <v>191</v>
-      </c>
-      <c r="H49" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>192</v>
-      </c>
-      <c r="B50" t="s">
-        <v>187</v>
-      </c>
-      <c r="C50">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="D50">
-        <v>2.1</v>
-      </c>
-      <c r="E50">
-        <v>1.4</v>
-      </c>
-      <c r="F50">
-        <v>2.5</v>
-      </c>
-      <c r="H50">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>192</v>
-      </c>
-      <c r="B51" t="s">
-        <v>188</v>
-      </c>
-      <c r="C51">
-        <v>4.3</v>
-      </c>
-      <c r="D51">
-        <v>2.5</v>
-      </c>
-      <c r="E51">
-        <v>3.5</v>
-      </c>
-      <c r="F51">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="H51">
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>192</v>
-      </c>
-      <c r="B52" t="s">
-        <v>189</v>
-      </c>
-      <c r="C52">
-        <v>15</v>
-      </c>
-      <c r="D52">
-        <v>13.4</v>
-      </c>
-      <c r="E52">
-        <v>15.2</v>
-      </c>
-      <c r="F52">
-        <v>18.5</v>
-      </c>
-      <c r="G52">
-        <v>12.5</v>
-      </c>
-      <c r="H52">
-        <v>10.8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>192</v>
-      </c>
-      <c r="B53" t="s">
-        <v>190</v>
-      </c>
-      <c r="C53">
-        <v>37.1</v>
-      </c>
-      <c r="D53">
-        <v>43</v>
-      </c>
-      <c r="E53">
-        <v>51.2</v>
-      </c>
-      <c r="F53">
-        <v>54</v>
-      </c>
-      <c r="G53">
-        <v>58.9</v>
-      </c>
-      <c r="H53">
-        <v>32.299999999999997</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>192</v>
-      </c>
-      <c r="B54">
-        <v>0</v>
-      </c>
-      <c r="C54">
-        <v>34.9</v>
-      </c>
-      <c r="D54">
-        <v>33</v>
-      </c>
-      <c r="E54">
-        <v>24.4</v>
-      </c>
-      <c r="F54">
-        <v>17.100000000000001</v>
-      </c>
-      <c r="G54">
-        <v>26.8</v>
-      </c>
-      <c r="H54">
-        <v>19.600000000000001</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>193</v>
-      </c>
-      <c r="C55">
-        <v>1317</v>
-      </c>
-      <c r="D55">
-        <v>1145</v>
-      </c>
-      <c r="E55">
-        <v>1170</v>
-      </c>
-      <c r="F55">
-        <v>855</v>
-      </c>
-      <c r="G55">
-        <v>56</v>
-      </c>
-      <c r="H55">
+      <c r="H55" s="2">
         <v>158</v>
       </c>
     </row>
@@ -5727,316 +5762,328 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42980F8A-CB6F-4C48-AF4B-C4BD3721079F}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="2"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C2" s="2">
+        <v>3646</v>
+      </c>
+      <c r="D2" s="2">
+        <v>5331</v>
+      </c>
+      <c r="E2" s="2">
+        <v>7649</v>
+      </c>
+      <c r="F2" s="2">
+        <v>110</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C3" s="2">
+        <v>3249</v>
+      </c>
+      <c r="D3" s="2">
+        <v>4664</v>
+      </c>
+      <c r="E3" s="2">
+        <v>6847</v>
+      </c>
+      <c r="F3" s="2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C4" s="2">
+        <v>4927</v>
+      </c>
+      <c r="D4" s="2">
+        <v>7289</v>
+      </c>
+      <c r="E4" s="2">
+        <v>10496</v>
+      </c>
+      <c r="F4" s="2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C5" s="2">
+        <v>11247</v>
+      </c>
+      <c r="D5" s="2">
+        <v>16023</v>
+      </c>
+      <c r="E5" s="2">
+        <v>21502</v>
+      </c>
+      <c r="F5" s="2">
+        <v>91</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C6" s="2">
+        <v>50</v>
+      </c>
+      <c r="D6" s="2">
+        <v>72</v>
+      </c>
+      <c r="E6" s="2">
+        <v>169</v>
+      </c>
+      <c r="F6" s="2">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C7" s="2">
+        <v>18025</v>
+      </c>
+      <c r="D7" s="2">
+        <v>27996</v>
+      </c>
+      <c r="E7" s="2">
+        <v>22279</v>
+      </c>
+      <c r="F7" s="2">
+        <v>24</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="F1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C9" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B2">
-        <v>3646</v>
-      </c>
-      <c r="C2">
-        <v>5331</v>
-      </c>
-      <c r="D2">
-        <v>7649</v>
-      </c>
-      <c r="E2">
-        <v>110</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="F9" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>205</v>
-      </c>
-      <c r="B3">
-        <v>3249</v>
-      </c>
-      <c r="C3">
-        <v>4664</v>
-      </c>
-      <c r="D3">
-        <v>6847</v>
-      </c>
-      <c r="E3">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>206</v>
-      </c>
-      <c r="B4">
-        <v>4927</v>
-      </c>
-      <c r="C4">
-        <v>7289</v>
-      </c>
-      <c r="D4">
-        <v>10496</v>
-      </c>
-      <c r="E4">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C10" s="2">
+        <v>28</v>
+      </c>
+      <c r="D10" s="2">
+        <v>20</v>
+      </c>
+      <c r="E10" s="2">
+        <v>29</v>
+      </c>
+      <c r="F10" s="2">
+        <v>31</v>
+      </c>
+      <c r="G10" s="2">
+        <v>33</v>
+      </c>
+      <c r="H10" s="2">
+        <v>39</v>
+      </c>
+      <c r="I10" s="2">
+        <v>24</v>
+      </c>
+      <c r="J10" s="2">
+        <v>27</v>
+      </c>
+      <c r="K10" s="2">
+        <v>34</v>
+      </c>
+      <c r="L10" s="2">
+        <v>32</v>
+      </c>
+      <c r="M10" s="2">
+        <v>16</v>
+      </c>
+      <c r="N10" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B5">
-        <v>11247</v>
-      </c>
-      <c r="C5">
-        <v>16023</v>
-      </c>
-      <c r="D5">
-        <v>21502</v>
-      </c>
-      <c r="E5">
-        <v>91</v>
-      </c>
-      <c r="F5" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C11" s="2">
+        <v>6</v>
+      </c>
+      <c r="D11" s="2">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2">
+        <v>13</v>
+      </c>
+      <c r="F11" s="2">
+        <v>11</v>
+      </c>
+      <c r="G11" s="2">
+        <v>15</v>
+      </c>
+      <c r="H11" s="2">
+        <v>15</v>
+      </c>
+      <c r="I11" s="2">
+        <v>14</v>
+      </c>
+      <c r="J11" s="2">
+        <v>20</v>
+      </c>
+      <c r="K11" s="2">
+        <v>13</v>
+      </c>
+      <c r="L11" s="2">
+        <v>3</v>
+      </c>
+      <c r="M11" s="2">
+        <v>13</v>
+      </c>
+      <c r="N11" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="B6">
-        <v>50</v>
-      </c>
-      <c r="C6">
-        <v>72</v>
-      </c>
-      <c r="D6">
-        <v>169</v>
-      </c>
-      <c r="E6">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="C12" s="2">
+        <v>18</v>
+      </c>
+      <c r="D12" s="2">
+        <v>9</v>
+      </c>
+      <c r="E12" s="2">
+        <v>15</v>
+      </c>
+      <c r="F12" s="2">
+        <v>19</v>
+      </c>
+      <c r="G12" s="2">
+        <v>19</v>
+      </c>
+      <c r="H12" s="2">
+        <v>15</v>
+      </c>
+      <c r="I12" s="2">
+        <v>16</v>
+      </c>
+      <c r="J12" s="2">
+        <v>14</v>
+      </c>
+      <c r="K12" s="2">
+        <v>13</v>
+      </c>
+      <c r="L12" s="2">
+        <v>14</v>
+      </c>
+      <c r="M12" s="2">
+        <v>10</v>
+      </c>
+      <c r="N12" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>211</v>
-      </c>
-      <c r="B7">
-        <v>18025</v>
-      </c>
-      <c r="C7">
-        <v>27996</v>
-      </c>
-      <c r="D7">
-        <v>22279</v>
-      </c>
-      <c r="E7">
-        <v>24</v>
-      </c>
-      <c r="F7" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C9" t="s">
-        <v>215</v>
-      </c>
-      <c r="D9" t="s">
-        <v>216</v>
-      </c>
-      <c r="E9" t="s">
-        <v>217</v>
-      </c>
-      <c r="F9" t="s">
-        <v>218</v>
-      </c>
-      <c r="G9" t="s">
-        <v>219</v>
-      </c>
-      <c r="H9" t="s">
-        <v>1</v>
-      </c>
-      <c r="I9" t="s">
-        <v>2</v>
-      </c>
-      <c r="J9" t="s">
-        <v>3</v>
-      </c>
-      <c r="K9" t="s">
-        <v>4</v>
-      </c>
-      <c r="L9" t="s">
-        <v>5</v>
-      </c>
-      <c r="M9" t="s">
-        <v>6</v>
-      </c>
-      <c r="N9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>214</v>
-      </c>
-      <c r="B10" t="s">
-        <v>221</v>
-      </c>
-      <c r="C10">
-        <v>28</v>
-      </c>
-      <c r="D10">
-        <v>20</v>
-      </c>
-      <c r="E10">
-        <v>29</v>
-      </c>
-      <c r="F10">
-        <v>31</v>
-      </c>
-      <c r="G10">
-        <v>33</v>
-      </c>
-      <c r="H10">
-        <v>39</v>
-      </c>
-      <c r="I10">
-        <v>24</v>
-      </c>
-      <c r="J10">
-        <v>27</v>
-      </c>
-      <c r="K10">
-        <v>34</v>
-      </c>
-      <c r="L10">
-        <v>32</v>
-      </c>
-      <c r="M10">
-        <v>16</v>
-      </c>
-      <c r="N10">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>214</v>
-      </c>
-      <c r="B11" t="s">
-        <v>222</v>
-      </c>
-      <c r="C11">
-        <v>6</v>
-      </c>
-      <c r="D11">
-        <v>8</v>
-      </c>
-      <c r="E11">
-        <v>13</v>
-      </c>
-      <c r="F11">
-        <v>11</v>
-      </c>
-      <c r="G11">
-        <v>15</v>
-      </c>
-      <c r="H11">
-        <v>15</v>
-      </c>
-      <c r="I11">
-        <v>14</v>
-      </c>
-      <c r="J11">
-        <v>20</v>
-      </c>
-      <c r="K11">
-        <v>13</v>
-      </c>
-      <c r="L11">
-        <v>3</v>
-      </c>
-      <c r="M11">
-        <v>13</v>
-      </c>
-      <c r="N11">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>214</v>
-      </c>
-      <c r="B12" t="s">
-        <v>223</v>
-      </c>
-      <c r="C12">
-        <v>18</v>
-      </c>
-      <c r="D12">
-        <v>9</v>
-      </c>
-      <c r="E12">
-        <v>15</v>
-      </c>
-      <c r="F12">
-        <v>19</v>
-      </c>
-      <c r="G12">
-        <v>19</v>
-      </c>
-      <c r="H12">
-        <v>15</v>
-      </c>
-      <c r="I12">
-        <v>16</v>
-      </c>
-      <c r="J12">
-        <v>14</v>
-      </c>
-      <c r="K12">
-        <v>13</v>
-      </c>
-      <c r="L12">
-        <v>14</v>
-      </c>
-      <c r="M12">
-        <v>10</v>
-      </c>
-      <c r="N12">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>